<commit_message>
added timings to SPI0 and  SD_HST
</commit_message>
<xml_diff>
--- a/SoMs/BW1099EMB/R1M0E1/BW1099EMB_R1M0E1_IO_TABLE.xlsx
+++ b/SoMs/BW1099EMB/R1M0E1/BW1099EMB_R1M0E1_IO_TABLE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrianLuxonis\Documents\GitHub\depthai-hardware\SoMs\BW1099EMB\R1M0E1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506AD847-30C2-4AD2-A099-DAA888E52A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0519C435-CFB2-41D9-A6F5-EF382E7B5B59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{2A677646-14BE-4F73-937F-BE4037A1016C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{2A677646-14BE-4F73-937F-BE4037A1016C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -222,9 +222,6 @@
     <t>3.3V GPIO</t>
   </si>
   <si>
-    <t xml:space="preserve">3.3V GPIO. Note PU/PD resistors that are configured for SDIO, but also compatible with SPI. </t>
-  </si>
-  <si>
     <t>CAMA_I2C_SDA</t>
   </si>
   <si>
@@ -327,15 +324,9 @@
     <t xml:space="preserve">USB UFP VBUS sense input for VBUS detect. Can be tied to 5V to enable Myriad X USB for embedded applications. </t>
   </si>
   <si>
-    <t xml:space="preserve">Configured for SDIO card detect, or as regular GPIO. Note 1.8V, 40.2k PU. </t>
-  </si>
-  <si>
     <t>SPI0_CS_1</t>
   </si>
   <si>
-    <t xml:space="preserve">GPIO, or can be configured as second CS for SPI0, MX in Controller or Peripheral mode. </t>
-  </si>
-  <si>
     <t>sd_hst0_clk</t>
   </si>
   <si>
@@ -345,9 +336,6 @@
     <t>SPI0_SIO0</t>
   </si>
   <si>
-    <t>Hardwired to 1099 on-board NOR DQ0</t>
-  </si>
-  <si>
     <t>sd_hst0_cmd</t>
   </si>
   <si>
@@ -360,9 +348,6 @@
     <t>SPI0_SIO1</t>
   </si>
   <si>
-    <t>Hardwired to 1099 on-board NOR DQ1</t>
-  </si>
-  <si>
     <t>CAM_B_D_PWM</t>
   </si>
   <si>
@@ -372,24 +357,15 @@
     <t>SPI0_SIO2</t>
   </si>
   <si>
-    <t>Hardwired to 1099 on-board NOR W#/DQ2</t>
-  </si>
-  <si>
     <t>Camera B reset/powerdown.</t>
   </si>
   <si>
     <t>SPI0_SIO3</t>
   </si>
   <si>
-    <t>Hardwired to 1099 on-board NOR DQ3/HOLD#</t>
-  </si>
-  <si>
     <t>PU: 1kR/1.8V</t>
   </si>
   <si>
-    <t>Hardwired to 1099 on-board NOR S#</t>
-  </si>
-  <si>
     <t>CAMB_CLK</t>
   </si>
   <si>
@@ -399,9 +375,6 @@
     <t>SPI0_SCK</t>
   </si>
   <si>
-    <t>Hardwired to 1099 on-board NOR C</t>
-  </si>
-  <si>
     <t>CAMB_I2C_SCL</t>
   </si>
   <si>
@@ -610,6 +583,33 @@
   </si>
   <si>
     <t>CAM_B_PWDN_N</t>
+  </si>
+  <si>
+    <t>3.3V GPIO. Note PU/PD resistors that are configured for SDIO, but also compatible with SPI. / +/-100ps inter-SD_HST</t>
+  </si>
+  <si>
+    <t>Configured for SDIO card detect, or as regular GPIO. Note 1.8V, 40.2k PU. / +/-100ps inter-SD_HST</t>
+  </si>
+  <si>
+    <t>GPIO, or can be configured as second CS for SPI0, MX in Controller or Peripheral mode. / +/-100ps inter-SPI0</t>
+  </si>
+  <si>
+    <t>Hardwired to 1099 on-board NOR DQ0 / +/-100ps inter-SPI0</t>
+  </si>
+  <si>
+    <t>Hardwired to 1099 on-board NOR DQ1 / +/-100ps inter-SPI0</t>
+  </si>
+  <si>
+    <t>Hardwired to 1099 on-board NOR W#/DQ2 / +/-100ps inter-SPI0</t>
+  </si>
+  <si>
+    <t>Hardwired to 1099 on-board NOR DQ3/HOLD# / +/-100ps inter-SPI0</t>
+  </si>
+  <si>
+    <t>Hardwired to 1099 on-board NOR S# / +/-100ps inter-SPI0</t>
+  </si>
+  <si>
+    <t>Hardwired to 1099 on-board NOR C / +/-100ps inter-SPI0</t>
   </si>
 </sst>
 </file>
@@ -1005,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A708E1D-7DB8-4706-8500-09B1FAE3DD99}">
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1022,7 +1022,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1042,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
@@ -1113,10 +1113,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>14</v>
@@ -1151,10 +1151,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C8" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>19</v>
@@ -1468,7 +1468,7 @@
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>51</v>
@@ -1524,10 +1524,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C34" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D34" t="s">
         <v>55</v>
@@ -1548,7 +1548,7 @@
         <v>60</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>61</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
@@ -1556,22 +1556,22 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" t="s">
+        <v>147</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C35" t="s">
-        <v>156</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="H35" t="s">
         <v>63</v>
-      </c>
-      <c r="H35" t="s">
-        <v>64</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
@@ -1579,10 +1579,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D36" s="1"/>
       <c r="H36" s="1"/>
@@ -1590,7 +1590,7 @@
         <v>16</v>
       </c>
       <c r="J36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
@@ -1598,20 +1598,20 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D37" s="1"/>
       <c r="H37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
@@ -1619,25 +1619,25 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C38" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" t="s">
         <v>70</v>
       </c>
-      <c r="E38" t="s">
+      <c r="H38" t="s">
         <v>71</v>
-      </c>
-      <c r="H38" t="s">
-        <v>72</v>
       </c>
       <c r="I38" t="s">
         <v>60</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>61</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
@@ -1645,17 +1645,17 @@
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D39" s="1"/>
       <c r="H39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="J39" t="s">
         <v>75</v>
-      </c>
-      <c r="J39" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
@@ -1663,28 +1663,28 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C40" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D40" t="s">
+        <v>76</v>
+      </c>
+      <c r="E40" t="s">
         <v>77</v>
       </c>
-      <c r="E40" t="s">
+      <c r="G40" t="s">
         <v>78</v>
       </c>
-      <c r="G40" t="s">
-        <v>79</v>
-      </c>
       <c r="H40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I40" t="s">
         <v>60</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>61</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
@@ -1692,17 +1692,17 @@
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D41" s="1"/>
       <c r="H41" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J41" t="s">
         <v>81</v>
-      </c>
-      <c r="J41" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
@@ -1710,31 +1710,31 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C42" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D42" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42" t="s">
         <v>83</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>84</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>85</v>
       </c>
-      <c r="G42" t="s">
-        <v>86</v>
-      </c>
       <c r="H42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I42" t="s">
         <v>60</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>61</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
@@ -1742,17 +1742,17 @@
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D43" s="1"/>
       <c r="H43" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J43" t="s">
         <v>88</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J43" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
@@ -1760,17 +1760,17 @@
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C44" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
@@ -1826,14 +1826,14 @@
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
@@ -1841,14 +1841,14 @@
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
@@ -1856,14 +1856,14 @@
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
@@ -1871,14 +1871,14 @@
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
@@ -1886,14 +1886,14 @@
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
@@ -1901,14 +1901,14 @@
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
@@ -1916,14 +1916,14 @@
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
@@ -1931,14 +1931,14 @@
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
@@ -1994,19 +1994,19 @@
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C61" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J61" t="s">
-        <v>96</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
@@ -2014,20 +2014,20 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C62" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D62" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J62" t="s">
-        <v>98</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.35">
@@ -2035,25 +2035,25 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C63" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D63" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E63" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I63" t="s">
         <v>60</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>61</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
@@ -2061,16 +2061,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C64" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>102</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
@@ -2078,28 +2078,28 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C65" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D65" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E65" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G65" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I65" t="s">
         <v>60</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>61</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
@@ -2107,16 +2107,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C66" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>107</v>
+        <v>186</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
@@ -2124,17 +2124,17 @@
         <v>65</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C67" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J67" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
@@ -2142,19 +2142,19 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C68" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>111</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
@@ -2162,17 +2162,17 @@
         <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C69" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J69" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
@@ -2180,19 +2180,19 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C70" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>114</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
@@ -2200,10 +2200,10 @@
         <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C71" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="H71" s="1"/>
       <c r="I71" s="1" t="s">
@@ -2216,19 +2216,19 @@
         <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C72" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>116</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
@@ -2262,10 +2262,10 @@
         <v>73</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C75" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>51</v>
@@ -2274,7 +2274,7 @@
         <v>16</v>
       </c>
       <c r="J75" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
@@ -2282,16 +2282,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C76" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
@@ -2323,19 +2323,19 @@
         <v>77</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C79" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H79" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J79" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
@@ -2343,22 +2343,22 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C80" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D80" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H80" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J80" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
@@ -2366,19 +2366,19 @@
         <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C81" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="H81" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J81" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
@@ -2386,22 +2386,22 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C82" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="D82" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H82" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J82" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
@@ -2435,7 +2435,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C85" s="1"/>
       <c r="H85" s="1"/>
@@ -2443,7 +2443,7 @@
         <v>12</v>
       </c>
       <c r="J85" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
@@ -2451,7 +2451,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C86" s="1"/>
       <c r="H86" s="1"/>
@@ -2459,7 +2459,7 @@
         <v>12</v>
       </c>
       <c r="J86" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
@@ -2467,7 +2467,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C87" s="1"/>
       <c r="H87" s="1"/>
@@ -2475,7 +2475,7 @@
         <v>12</v>
       </c>
       <c r="J87" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
@@ -2483,7 +2483,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C88" s="1"/>
       <c r="H88" s="1"/>
@@ -2491,7 +2491,7 @@
         <v>12</v>
       </c>
       <c r="J88" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
@@ -2525,7 +2525,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C91" s="1"/>
       <c r="H91" s="1"/>
@@ -2533,7 +2533,7 @@
         <v>12</v>
       </c>
       <c r="J91" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.35">
@@ -2541,7 +2541,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C92" s="1"/>
       <c r="H92" s="1"/>
@@ -2549,7 +2549,7 @@
         <v>12</v>
       </c>
       <c r="J92" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.35">
@@ -2557,7 +2557,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C93" s="1"/>
       <c r="H93" s="1"/>
@@ -2565,7 +2565,7 @@
         <v>12</v>
       </c>
       <c r="J93" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.35">
@@ -2573,7 +2573,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C94" s="1"/>
       <c r="H94" s="1"/>
@@ -2581,7 +2581,7 @@
         <v>12</v>
       </c>
       <c r="J94" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.35">
@@ -2615,7 +2615,7 @@
         <v>95</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C97" s="1"/>
       <c r="H97" s="1"/>
@@ -2623,7 +2623,7 @@
         <v>12</v>
       </c>
       <c r="J97" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.35">
@@ -2631,7 +2631,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C98" s="1"/>
       <c r="H98" s="1"/>
@@ -2639,7 +2639,7 @@
         <v>12</v>
       </c>
       <c r="J98" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.35">
@@ -2647,7 +2647,7 @@
         <v>97</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C99" s="1"/>
       <c r="H99" s="1"/>
@@ -2655,7 +2655,7 @@
         <v>12</v>
       </c>
       <c r="J99" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.35">
@@ -2663,7 +2663,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C100" s="1"/>
       <c r="H100" s="1"/>
@@ -2671,7 +2671,7 @@
         <v>12</v>
       </c>
       <c r="J100" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated data sheet and io table for BW1099EMB
</commit_message>
<xml_diff>
--- a/SoMs/BW1099EMB/R1M0E1/BW1099EMB_R1M0E1_IO_TABLE.xlsx
+++ b/SoMs/BW1099EMB/R1M0E1/BW1099EMB_R1M0E1_IO_TABLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrianLuxonis\Desktop\hardware\Luxonis_HW_Documentation\BW1099EMB Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD183C41-00A9-4A0C-8BDB-7059C4BD22BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A0CDA8-54F0-4E6D-ABE1-19F4F4BC65DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11020" yWindow="6460" windowWidth="24570" windowHeight="17130" xr2:uid="{2A677646-14BE-4F73-937F-BE4037A1016C}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{2A677646-14BE-4F73-937F-BE4037A1016C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1009,11 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A708E1D-7DB8-4706-8500-09B1FAE3DD99}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H115" sqref="H115"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1073,7 +1072,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1086,7 +1085,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1141,7 +1140,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1182,7 +1181,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1194,7 +1193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1206,7 +1205,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1221,7 +1220,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1236,7 +1235,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1251,7 +1250,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1266,7 +1265,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1278,7 +1277,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1290,7 +1289,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1305,7 +1304,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1320,7 +1319,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1335,7 +1334,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1350,7 +1349,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1362,7 +1361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1374,7 +1373,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1389,7 +1388,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1404,7 +1403,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1419,7 +1418,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1434,7 +1433,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1446,7 +1445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1458,7 +1457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1493,7 +1492,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1508,7 +1507,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1520,7 +1519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1532,7 +1531,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>40</v>
       </c>
@@ -1627,7 +1626,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>61</v>
       </c>
@@ -1653,7 +1652,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1671,7 +1670,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>63</v>
       </c>
@@ -1700,7 +1699,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1718,7 +1717,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>32</v>
       </c>
@@ -1750,7 +1749,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1786,7 +1785,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1798,7 +1797,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1810,7 +1809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1822,7 +1821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1834,7 +1833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1849,7 +1848,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1864,7 +1863,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1879,7 +1878,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1894,7 +1893,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1909,7 +1908,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1924,7 +1923,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1939,7 +1938,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1954,7 +1953,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1966,7 +1965,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1978,7 +1977,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1990,7 +1989,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2043,7 +2042,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>36</v>
       </c>
@@ -2086,7 +2085,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>38</v>
       </c>
@@ -2248,7 +2247,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2261,7 +2260,7 @@
       </c>
       <c r="J73" s="1"/>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2311,7 +2310,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2323,7 +2322,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2366,7 +2365,7 @@
         <v>173</v>
       </c>
       <c r="D80" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="H80" t="s">
         <v>62</v>
@@ -2375,7 +2374,7 @@
         <v>15</v>
       </c>
       <c r="J80" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
@@ -2409,7 +2408,7 @@
         <v>175</v>
       </c>
       <c r="D82" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="H82" t="s">
         <v>62</v>
@@ -2418,10 +2417,10 @@
         <v>15</v>
       </c>
       <c r="J82" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2434,7 +2433,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2447,7 +2446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2463,7 +2462,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2479,7 +2478,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2495,7 +2494,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2511,7 +2510,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2524,7 +2523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2537,7 +2536,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2553,7 +2552,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2569,7 +2568,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2585,7 +2584,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2601,7 +2600,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2614,7 +2613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -2627,7 +2626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -2643,7 +2642,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -2659,7 +2658,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -2675,7 +2674,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -2691,7 +2690,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -2704,7 +2703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -2725,16 +2724,7 @@
       <c r="I103" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:J102" xr:uid="{66DCD8A4-7681-4B36-987C-6CF98CBE9C65}">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="1.8V GPIO"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:J82">
-      <sortCondition ref="A2:A102"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A2:J102" xr:uid="{66DCD8A4-7681-4B36-987C-6CF98CBE9C65}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>

</xml_diff>